<commit_message>
Conceptual model for EE dis
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/IO_Ghana/Database/Expanding/Concordance/C_EORA.xlsx
+++ b/CIVICS_Ghana/IO_Ghana/Database/Expanding/Concordance/C_EORA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS\CIVICS_Ghana\IO_Ghana\Database\Expanding\Concordance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568CF252-5430-4F2F-A519-7731DFDB0581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4659AED-A5FF-4530-8160-A9B1648D888B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,11 +701,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B128D3-0D2A-4987-9C35-519F4FC4CCEF}">
   <dimension ref="A1:BD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV10" sqref="AV10"/>
+      <selection pane="bottomRight" activeCell="BB24" sqref="BB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2875,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="AP13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ13" s="1">
         <v>0</v>
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="BD13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.3">
@@ -3397,7 +3397,7 @@
         <v>0</v>
       </c>
       <c r="AT16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU16" s="1">
         <v>0</v>
@@ -3427,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="BD16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.3">
@@ -4432,7 +4432,7 @@
         <v>1</v>
       </c>
       <c r="AY22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ22" s="1">
         <v>1</v>
@@ -5112,7 +5112,7 @@
         <v>0</v>
       </c>
       <c r="AY26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ26" s="1">
         <v>0</v>

</xml_diff>